<commit_message>
Deploying to gh-pages from @ samply/bbmri-fhir-ig@2175841b2443349fa9e69ee77ed705e5df4b08f4 🚀
</commit_message>
<xml_diff>
--- a/CodeSystem-BiobankCapabilities.xlsx
+++ b/CodeSystem-BiobankCapabilities.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-02-08T10:28:33+00:00</t>
+    <t>2023-09-01T08:46:52+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -308,10 +308,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyBorder="true" applyFill="true" applyFont="true">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true" applyFont="true">
       <alignment vertical="top" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment vertical="top" wrapText="true"/>
     </xf>
   </cellXfs>

</xml_diff>